<commit_message>
CPU functions was implemeted.
</commit_message>
<xml_diff>
--- a/annotation/WEBVM - OPCODES.xlsx
+++ b/annotation/WEBVM - OPCODES.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
   <si>
     <t xml:space="preserve">WEBVM – OPCODES</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">REGISTER</t>
   </si>
   <si>
-    <t xml:space="preserve">ldx 0x0000 $13</t>
+    <t xml:space="preserve">ldx 0x00 $13</t>
   </si>
   <si>
     <t xml:space="preserve">READ DATA FROM THE INDICATED ADDRESS AND STORE IN INDICATED REGISTER.</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">00000010</t>
   </si>
   <si>
-    <t xml:space="preserve">stx $13 0x0000</t>
+    <t xml:space="preserve">stx $13 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">STORE FROM INDICATED REGISTER INTO THE INDICATED ADDRESS.</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">00001000</t>
   </si>
   <si>
-    <t xml:space="preserve">jmp 0x0000</t>
+    <t xml:space="preserve">jmp 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">JUMP TO THE INDICATED ADDRESS</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">00001001</t>
   </si>
   <si>
-    <t xml:space="preserve">jsr 0x0000</t>
+    <t xml:space="preserve">jsr 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">JUMP TO THE INDICATED ADDRESS AND STORES CURRENT ADDRESS ON STACK FOR RETURN AFTER FINISHED PROCESS.</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">00001100</t>
   </si>
   <si>
-    <t xml:space="preserve">beg 0x0000 0x0000</t>
+    <t xml:space="preserve">beg 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “EQUALS”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">00001101</t>
   </si>
   <si>
-    <t xml:space="preserve">bne 0x0000 0x0000</t>
+    <t xml:space="preserve">bne 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “NOT EQUALS”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">00001110</t>
   </si>
   <si>
-    <t xml:space="preserve">bgt 0x0000 0x0000</t>
+    <t xml:space="preserve">bgt 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “GREAT THEN”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">00001111</t>
   </si>
   <si>
-    <t xml:space="preserve">blt 0x0000 0x0000</t>
+    <t xml:space="preserve">blt 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “LESS THEN”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">00010000</t>
   </si>
   <si>
-    <t xml:space="preserve">bge 0x0000 0x0000</t>
+    <t xml:space="preserve">bge 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “GREAT THEN EQUALS”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">00010001</t>
   </si>
   <si>
-    <t xml:space="preserve">ble 0x0000 0x0000</t>
+    <t xml:space="preserve">ble 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">COMPARE IF THE VALUE IN REGISTERS  CHOSEN BY CMP COMMAND IS “LESS THEN EQUALS”. IF TRUE, THE CPU WILL JUMP TO THE FIRST ADDRESS, IF FALSE, THE CPU WILL JUMP TO THE SECOND ADDRESS</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">not $10 $24</t>
   </si>
   <si>
-    <t xml:space="preserve">MAKES LOGICAL “NOT” OPERATION BETWEEN REGISTERS. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
+    <t xml:space="preserve">MAKES LOGICAL “NOT” OPERATION WITH FIRST INDICATED REGISTER. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
   </si>
   <si>
     <t xml:space="preserve">NAND</t>
@@ -394,10 +394,26 @@
     <t xml:space="preserve">00011100</t>
   </si>
   <si>
-    <t xml:space="preserve">rol $10 $28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO SHIFT LEFT BETWEEN INDICATED REGISTER.</t>
+    <t xml:space="preserve">rol $10 $23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DO SHIFT LEFT ON INDICATED REGISTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ROR</t>
@@ -409,7 +425,47 @@
     <t xml:space="preserve">ror $4 $12</t>
   </si>
   <si>
-    <t xml:space="preserve">DO SHIFT RIGHT BETWEEN INDICATED REGISTER.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DO SHIFT RIGHT INDICATED REGISTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prt 0xaa 0xff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT BYTES BETWEEN INDICATED ADDRESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inp 0x0a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPTURE INPUT OF USER AT THERE PRESS ENTER.</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTERS</t>
@@ -430,7 +486,7 @@
     <t xml:space="preserve">$31</t>
   </si>
   <si>
-    <t xml:space="preserve">64 BITS EACH</t>
+    <t xml:space="preserve">8 BITS EACH</t>
   </si>
 </sst>
 </file>
@@ -445,7 +501,7 @@
     <numFmt numFmtId="168" formatCode="[$-409]@"/>
     <numFmt numFmtId="169" formatCode="&quot;[$]&quot;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -487,6 +543,11 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -727,7 +788,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,13 +898,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
@@ -1455,7 +1516,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
@@ -1476,7 +1537,7 @@
       </c>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>126</v>
       </c>
@@ -1497,57 +1558,97 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="33" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
+      <c r="B33" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="C33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="F33" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B34" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="38">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1580,10 +1681,12 @@
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
First version is done
</commit_message>
<xml_diff>
--- a/annotation/WEBVM - OPCODES.xlsx
+++ b/annotation/WEBVM - OPCODES.xlsx
@@ -397,23 +397,7 @@
     <t xml:space="preserve">rol $10 $23</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">DO SHIFT LEFT ON INDICATED REGISTER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
-    </r>
+    <t xml:space="preserve">DO SHIFT LEFT ON INDICATED REGISTER. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
   </si>
   <si>
     <t xml:space="preserve">ROR</t>
@@ -425,23 +409,7 @@
     <t xml:space="preserve">ror $4 $12</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">DO SHIFT RIGHT INDICATED REGISTER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
-    </r>
+    <t xml:space="preserve">DO SHIFT RIGHT INDICATED REGISTER. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST  INDICATED REGISTER.</t>
   </si>
   <si>
     <t xml:space="preserve">PRT</t>
@@ -501,7 +469,7 @@
     <numFmt numFmtId="168" formatCode="[$-409]@"/>
     <numFmt numFmtId="169" formatCode="&quot;[$]&quot;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -543,11 +511,6 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -788,7 +751,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -901,10 +864,10 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>

</xml_diff>